<commit_message>
new project and main code
</commit_message>
<xml_diff>
--- a/Documentation/nrf51822-button.xlsx
+++ b/Documentation/nrf51822-button.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="120" windowWidth="28800" windowHeight="17240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="nrf51822-button.csv" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="132">
   <si>
     <t>Qty</t>
   </si>
@@ -284,9 +284,6 @@
     <t>0.895 x 0.790</t>
   </si>
   <si>
-    <t>Assembly cost</t>
-  </si>
-  <si>
     <t>3.9p</t>
   </si>
   <si>
@@ -302,21 +299,6 @@
     <t>490-1303-1-ND</t>
   </si>
   <si>
-    <t>0603 cap (bypass)</t>
-  </si>
-  <si>
-    <t>0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>C1608C0G1E472J080AA</t>
-  </si>
-  <si>
-    <t>445-2712-1-ND</t>
-  </si>
-  <si>
     <t>Ext Cost 1 Board</t>
   </si>
   <si>
@@ -387,6 +369,57 @@
   </si>
   <si>
     <t>Xtal</t>
+  </si>
+  <si>
+    <t>Light Pipe</t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>492-1531-ND</t>
+  </si>
+  <si>
+    <t>PLP5-2-125</t>
+  </si>
+  <si>
+    <t>Bivar Inc</t>
+  </si>
+  <si>
+    <t>LIGHT PIPE PNL 5MM LENS 0.125"</t>
+  </si>
+  <si>
+    <t>0402 cap (bypass)</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>C0402C473K4RACTU</t>
+  </si>
+  <si>
+    <t>399-3519-1-ND</t>
+  </si>
+  <si>
+    <t>1490-1038-ND</t>
+  </si>
+  <si>
+    <t>NRF51-DK</t>
+  </si>
+  <si>
+    <t>DEV KIT FOR NRF51 SERIES</t>
+  </si>
+  <si>
+    <t>490-4982-ND</t>
+  </si>
+  <si>
+    <t>MXHS83QE3000</t>
+  </si>
+  <si>
+    <t>CONN MEAS PROBE FOR SWD/SWF CONN</t>
+  </si>
+  <si>
+    <t>Programing and Development Tools</t>
   </si>
 </sst>
 </file>
@@ -443,8 +476,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,7 +569,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -535,6 +596,20 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -561,6 +636,20 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -890,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -945,10 +1034,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="13">
@@ -983,7 +1072,7 @@
         <v>0.46</v>
       </c>
       <c r="K2" s="3">
-        <f t="shared" ref="K2:K23" si="0">A2*I2</f>
+        <f t="shared" ref="K2:K21" si="0">A2*I2</f>
         <v>0.64</v>
       </c>
       <c r="L2" s="3">
@@ -1027,7 +1116,7 @@
         <v>0.2</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L23" si="1">A3*J3</f>
+        <f t="shared" ref="L3:L21" si="1">A3*J3</f>
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
@@ -1076,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
@@ -1091,10 +1180,10 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
         <v>88</v>
-      </c>
-      <c r="H5" t="s">
-        <v>89</v>
       </c>
       <c r="I5" s="3">
         <v>0.2</v>
@@ -1119,7 +1208,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -1159,7 +1248,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -1171,10 +1260,10 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" t="s">
         <v>90</v>
-      </c>
-      <c r="H7" t="s">
-        <v>91</v>
       </c>
       <c r="I7" s="3">
         <v>0.1</v>
@@ -1199,7 +1288,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -1239,22 +1328,22 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="I9" s="3">
         <v>0.24</v>
@@ -1279,7 +1368,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -1288,13 +1377,13 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I10" s="3">
         <v>0.1</v>
@@ -1319,7 +1408,7 @@
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
         <v>42</v>
@@ -1359,36 +1448,36 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="H12" t="s">
+        <v>99</v>
       </c>
       <c r="I12" s="3">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J12" s="3">
-        <v>4.99E-2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" ref="K12" si="2">A12*I12</f>
-        <v>0.15</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" ref="L12" si="3">A12*J12</f>
-        <v>4.99E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="13">
@@ -1396,39 +1485,39 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="I13" s="3">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>0.1169</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1169</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="13">
@@ -1436,10 +1525,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
@@ -1451,10 +1540,10 @@
         <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I14" s="3">
         <v>0.18</v>
@@ -1476,10 +1565,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
         <v>49</v>
@@ -1491,24 +1580,24 @@
         <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I15" s="3">
-        <v>0.18</v>
+        <v>0.43</v>
       </c>
       <c r="J15" s="3">
-        <v>0.1169</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.43</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="1"/>
-        <v>0.1169</v>
+        <v>0.28100000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="13">
@@ -1516,93 +1605,93 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I16" s="3">
-        <v>0.43</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J16" s="3">
-        <v>0.28100000000000003</v>
+        <v>1.22</v>
       </c>
       <c r="K16" s="3">
         <f t="shared" si="0"/>
-        <v>0.43</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="1"/>
-        <v>0.28100000000000003</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="13">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="I17" s="3">
-        <v>2.2000000000000002</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="J17" s="3">
-        <v>1.22</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>0.249</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="1"/>
-        <v>1.22</v>
+        <v>7.6499999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="13">
       <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" s="5">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
@@ -1611,10 +1700,10 @@
         <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I18" s="3">
         <v>8.3000000000000004E-2</v>
@@ -1624,51 +1713,51 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="0"/>
-        <v>0.249</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" si="1"/>
-        <v>7.6499999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="13">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="I19" s="3">
-        <v>8.3000000000000004E-2</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="J19" s="3">
-        <v>2.5499999999999998E-2</v>
+        <v>3.0139999999999998</v>
       </c>
       <c r="K19" s="3">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="L19" s="3">
         <f t="shared" si="1"/>
-        <v>5.0999999999999997E-2</v>
+        <v>3.0139999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="13">
@@ -1676,40 +1765,30 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>74</v>
+        <v>120</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="3">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="J20" s="3">
-        <v>3.0139999999999998</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="0"/>
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="L20" s="3">
-        <f t="shared" si="1"/>
-        <v>3.0139999999999998</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" ht="13">
       <c r="A21">
@@ -1719,7 +1798,7 @@
         <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
         <v>79</v>
@@ -1782,61 +1861,147 @@
         <v>1.1784166666666667</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="0"/>
+        <f>A22*I22</f>
         <v>1.1784166666666667</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" si="1"/>
+        <f>A22*J22</f>
         <v>1.1784166666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="13">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+    <row r="23" spans="1:12" customFormat="1" ht="13"/>
+    <row r="24" spans="1:12" ht="13">
+      <c r="A24"/>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="4">
-        <f>SUM(K2:K23)</f>
-        <v>12.283416666666668</v>
-      </c>
-      <c r="L24" s="4">
-        <f>SUM(L2:L23)</f>
-        <v>53.291316666666688</v>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" ht="13">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H25" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="3">
+        <v>76.569999999999993</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3">
+        <f t="shared" ref="K25:L27" si="2">A25*I25</f>
+        <v>76.569999999999993</v>
+      </c>
+      <c r="L25" s="3">
+        <v>76.569999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26" s="3">
+        <v>8.89</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3">
+        <f t="shared" si="2"/>
+        <v>8.89</v>
+      </c>
+      <c r="L26" s="3">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="3">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
+        <f t="shared" si="2"/>
+        <v>37.630000000000003</v>
+      </c>
+      <c r="L27" s="3">
+        <v>37.630000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="4">
+        <f>SUM(K2:K27)</f>
+        <v>135.22341666666668</v>
+      </c>
+      <c r="L29" s="4">
+        <f>SUM(L2:L27)</f>
+        <v>176.33141666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>